<commit_message>
Final version for step 1
There were some duplicate rown in the excel file, which I have deleted
</commit_message>
<xml_diff>
--- a/RESULTS/Round1/_free_text_answers_agreed.xlsx
+++ b/RESULTS/Round1/_free_text_answers_agreed.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4548" uniqueCount="1286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4525" uniqueCount="1287">
   <si>
     <t>index</t>
   </si>
@@ -3882,7 +3882,10 @@
     <t>rule categories matched</t>
   </si>
   <si>
-    <t>Letter rule expained with "numbers"</t>
+    <t>color-blindess question distracted him</t>
+  </si>
+  <si>
+    <t>Letter rule expained with numbers</t>
   </si>
 </sst>
 </file>
@@ -3927,7 +3930,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3952,6 +3955,12 @@
         <bgColor theme="6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3972,7 +3981,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4023,9 +4032,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -4253,11 +4265,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O563"/>
+  <dimension ref="A1:P560"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <pane ySplit="1" topLeftCell="A542" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q546" sqref="Q546"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4302,14 +4314,14 @@
         <v>1268</v>
       </c>
       <c r="L1" s="24" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>1284</v>
       </c>
       <c r="N1" s="8">
         <f>SUM(M:M)</f>
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>8</v>
@@ -8230,7 +8242,7 @@
       <c r="E96" s="11">
         <v>5</v>
       </c>
-      <c r="F96" s="2" t="s">
+      <c r="F96" s="22" t="s">
         <v>588</v>
       </c>
       <c r="G96" s="11" t="s">
@@ -8330,6 +8342,9 @@
       <c r="K98" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L98">
+        <v>1</v>
+      </c>
       <c r="M98" s="11">
         <f>IF(I98=J98,1,0)</f>
         <v>0</v>
@@ -12755,6 +12770,9 @@
       <c r="K205" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L205">
+        <v>1</v>
+      </c>
       <c r="M205" s="11">
         <f>IF(I205=J205,1,0)</f>
         <v>0</v>
@@ -14870,7 +14888,7 @@
       </c>
       <c r="O256" s="11"/>
     </row>
-    <row r="257" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A257" s="11">
         <v>442</v>
       </c>
@@ -14913,7 +14931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A258" s="11">
         <v>443</v>
       </c>
@@ -14954,7 +14972,7 @@
       </c>
       <c r="O258" s="11"/>
     </row>
-    <row r="259" spans="1:15" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:16" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A259" s="11">
         <v>444</v>
       </c>
@@ -14994,7 +15012,7 @@
       </c>
       <c r="O259" s="11"/>
     </row>
-    <row r="260" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A260" s="11">
         <v>446</v>
       </c>
@@ -15035,7 +15053,7 @@
       </c>
       <c r="O260" s="11"/>
     </row>
-    <row r="261" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A261" s="11">
         <v>447</v>
       </c>
@@ -15076,7 +15094,7 @@
       </c>
       <c r="O261" s="11"/>
     </row>
-    <row r="262" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A262" s="11">
         <v>448</v>
       </c>
@@ -15116,7 +15134,7 @@
       </c>
       <c r="O262" s="11"/>
     </row>
-    <row r="263" spans="1:15" ht="174" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:16" ht="174" x14ac:dyDescent="0.35">
       <c r="A263" s="11">
         <v>449</v>
       </c>
@@ -15158,8 +15176,11 @@
       <c r="O263" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="264" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="P263" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A264" s="11">
         <v>452</v>
       </c>
@@ -15200,7 +15221,7 @@
       </c>
       <c r="O264" s="11"/>
     </row>
-    <row r="265" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A265" s="11">
         <v>453</v>
       </c>
@@ -15241,7 +15262,7 @@
       </c>
       <c r="O265" s="11"/>
     </row>
-    <row r="266" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A266" s="11">
         <v>454</v>
       </c>
@@ -15282,7 +15303,7 @@
       </c>
       <c r="O266" s="11"/>
     </row>
-    <row r="267" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A267" s="11">
         <v>455</v>
       </c>
@@ -15323,7 +15344,7 @@
       </c>
       <c r="O267" s="11"/>
     </row>
-    <row r="268" spans="1:15" ht="87" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:16" ht="87" x14ac:dyDescent="0.35">
       <c r="A268" s="11">
         <v>456</v>
       </c>
@@ -15366,7 +15387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A269" s="11">
         <v>457</v>
       </c>
@@ -15409,7 +15430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A270" s="11">
         <v>458</v>
       </c>
@@ -15450,7 +15471,7 @@
       </c>
       <c r="O270" s="11"/>
     </row>
-    <row r="271" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A271" s="11">
         <v>461</v>
       </c>
@@ -15491,7 +15512,7 @@
       </c>
       <c r="O271" s="11"/>
     </row>
-    <row r="272" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A272" s="11">
         <v>462</v>
       </c>
@@ -15925,7 +15946,7 @@
       <c r="E282" s="11">
         <v>5</v>
       </c>
-      <c r="F282" s="2" t="s">
+      <c r="F282" s="22" t="s">
         <v>288</v>
       </c>
       <c r="G282" s="11" t="s">
@@ -16107,6 +16128,9 @@
       <c r="K286" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L286">
+        <v>1</v>
+      </c>
       <c r="M286" s="11">
         <f>IF(I286=J286,1,0)</f>
         <v>0</v>
@@ -18182,6 +18206,9 @@
       <c r="K336" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L336">
+        <v>1</v>
+      </c>
       <c r="M336" s="11">
         <f>IF(I336=J336,1,0)</f>
         <v>0</v>
@@ -21783,6 +21810,9 @@
         <f>IF(I423=J423,I423)</f>
         <v>L</v>
       </c>
+      <c r="L423">
+        <v>1</v>
+      </c>
       <c r="M423" s="11">
         <f>IF(I423=J423,1,0)</f>
         <v>1</v>
@@ -25245,7 +25275,7 @@
       <c r="H507" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="I507" s="11" t="s">
+      <c r="I507" s="20" t="s">
         <v>20</v>
       </c>
       <c r="J507" s="11" t="s">
@@ -25377,6 +25407,9 @@
       <c r="K510" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L510">
+        <v>1</v>
+      </c>
       <c r="M510" s="11">
         <f>IF(I510=J510,1,0)</f>
         <v>0</v>
@@ -26200,6 +26233,9 @@
       <c r="K530" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="L530">
+        <v>1</v>
+      </c>
       <c r="M530" s="11">
         <f>IF(I530=J530,1,0)</f>
         <v>0</v>
@@ -26209,10 +26245,10 @@
       </c>
     </row>
     <row r="531" spans="1:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A531" s="11">
+      <c r="A531" s="20">
         <v>888</v>
       </c>
-      <c r="B531" s="11" t="s">
+      <c r="B531" s="20" t="s">
         <v>561</v>
       </c>
       <c r="C531" s="11" t="s">
@@ -26221,16 +26257,16 @@
       <c r="D531" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E531" s="11">
+      <c r="E531" s="20">
         <v>7</v>
       </c>
-      <c r="F531" s="2" t="s">
+      <c r="F531" s="22" t="s">
         <v>735</v>
       </c>
-      <c r="G531" s="11" t="s">
+      <c r="G531" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H531" s="2" t="s">
+      <c r="H531" s="22" t="s">
         <v>736</v>
       </c>
       <c r="I531" s="11" t="s">
@@ -26414,10 +26450,10 @@
       <c r="O535" s="11"/>
     </row>
     <row r="536" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A536" s="11">
+      <c r="A536" s="20">
         <v>896</v>
       </c>
-      <c r="B536" s="11" t="s">
+      <c r="B536" s="20" t="s">
         <v>898</v>
       </c>
       <c r="C536" s="11" t="s">
@@ -26426,16 +26462,16 @@
       <c r="D536" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E536" s="11">
+      <c r="E536" s="20">
         <v>3</v>
       </c>
-      <c r="F536" s="2" t="s">
+      <c r="F536" s="22" t="s">
         <v>1059</v>
       </c>
-      <c r="G536" s="11" t="s">
+      <c r="G536" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="H536" s="2" t="s">
+      <c r="H536" s="22" t="s">
         <v>1060</v>
       </c>
       <c r="I536" s="11" t="s">
@@ -26455,10 +26491,10 @@
       <c r="O536" s="11"/>
     </row>
     <row r="537" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A537" s="11">
+      <c r="A537" s="20">
         <v>898</v>
       </c>
-      <c r="B537" s="11" t="s">
+      <c r="B537" s="20" t="s">
         <v>737</v>
       </c>
       <c r="C537" s="11" t="s">
@@ -26467,16 +26503,16 @@
       <c r="D537" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E537" s="11">
+      <c r="E537" s="20">
         <v>7</v>
       </c>
-      <c r="F537" s="2" t="s">
+      <c r="F537" s="22" t="s">
         <v>888</v>
       </c>
-      <c r="G537" s="11" t="s">
+      <c r="G537" s="20" t="s">
         <v>890</v>
       </c>
-      <c r="H537" s="2" t="s">
+      <c r="H537" s="22" t="s">
         <v>889</v>
       </c>
       <c r="I537" s="11" t="s">
@@ -26703,10 +26739,10 @@
       <c r="O542" s="11"/>
     </row>
     <row r="543" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A543" s="11">
+      <c r="A543" s="18">
         <v>915</v>
       </c>
-      <c r="B543" s="11" t="s">
+      <c r="B543" s="18" t="s">
         <v>737</v>
       </c>
       <c r="C543" s="11" t="s">
@@ -26715,16 +26751,16 @@
       <c r="D543" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E543" s="11">
+      <c r="E543" s="18">
         <v>10</v>
       </c>
-      <c r="F543" s="2" t="s">
+      <c r="F543" s="21" t="s">
         <v>893</v>
       </c>
-      <c r="G543" s="11" t="s">
+      <c r="G543" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H543" s="2" t="s">
+      <c r="H543" s="21" t="s">
         <v>894</v>
       </c>
       <c r="I543" s="11" t="s">
@@ -26744,10 +26780,10 @@
       <c r="O543" s="11"/>
     </row>
     <row r="544" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A544" s="20">
+      <c r="A544" s="18">
         <v>916</v>
       </c>
-      <c r="B544" s="20" t="s">
+      <c r="B544" s="18" t="s">
         <v>737</v>
       </c>
       <c r="C544" s="11" t="s">
@@ -26756,16 +26792,16 @@
       <c r="D544" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E544" s="20">
+      <c r="E544" s="18">
         <v>7</v>
       </c>
-      <c r="F544" s="22" t="s">
+      <c r="F544" s="21" t="s">
         <v>895</v>
       </c>
-      <c r="G544" s="20" t="s">
+      <c r="G544" s="18" t="s">
         <v>897</v>
       </c>
-      <c r="H544" s="22" t="s">
+      <c r="H544" s="21" t="s">
         <v>896</v>
       </c>
       <c r="I544" s="11" t="s">
@@ -26904,12 +26940,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="548" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="548" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A548" s="13">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B548" s="13" t="s">
-        <v>1066</v>
+        <v>199</v>
       </c>
       <c r="C548" s="11" t="s">
         <v>11</v>
@@ -26918,233 +26954,156 @@
         <v>11</v>
       </c>
       <c r="E548" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F548" s="16" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="G548" s="13" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="H548" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="I548" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J548" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K548" s="4" t="str">
+        <v>1282</v>
+      </c>
+      <c r="I548" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J548" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K548" s="25" t="str">
         <f>IF(I548=J548,I548)</f>
-        <v>N</v>
-      </c>
+        <v>L</v>
+      </c>
+      <c r="L548" s="25"/>
       <c r="M548" s="11">
         <f>IF(I548=J548,1,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="549" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="549" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A549" s="13">
-        <v>912</v>
+        <v>932</v>
       </c>
       <c r="B549" s="13" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C549" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D549" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E549" s="13">
+        <v>10</v>
+      </c>
+      <c r="F549" s="16" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G549" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H549" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="I549" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J549" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K549" s="26" t="str">
+        <f>IF(I549=J549,I549)</f>
+        <v>N</v>
+      </c>
+      <c r="L549" s="27"/>
+      <c r="M549" s="11">
+        <f>IF(I549=J549,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A550" s="13">
+        <v>933</v>
+      </c>
+      <c r="B550" s="13" t="s">
         <v>737</v>
       </c>
-      <c r="C549" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D549" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E549" s="13">
+      <c r="C550" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D550" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E550" s="13">
         <v>7</v>
       </c>
-      <c r="F549" s="16" t="s">
-        <v>891</v>
-      </c>
-      <c r="G549" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H549" s="16" t="s">
-        <v>892</v>
-      </c>
-      <c r="I549" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="J549" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="K549" s="4" t="str">
-        <f>IF(I549=J549,I549)</f>
-        <v>S</v>
-      </c>
-      <c r="M549" s="11">
-        <f t="shared" ref="M549:M553" si="0">IF(I549=J549,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="550" spans="1:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="A550" s="13">
-        <v>913</v>
-      </c>
-      <c r="B550" s="13" t="s">
-        <v>898</v>
-      </c>
-      <c r="C550" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D550" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E550" s="13">
-        <v>2</v>
-      </c>
       <c r="F550" s="16" t="s">
-        <v>1064</v>
+        <v>1283</v>
       </c>
       <c r="G550" s="13" t="s">
         <v>130</v>
       </c>
       <c r="H550" s="16" t="s">
-        <v>1065</v>
-      </c>
-      <c r="I550" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="J550" s="11" t="s">
-        <v>571</v>
-      </c>
-      <c r="K550" s="4" t="str">
+        <v>398</v>
+      </c>
+      <c r="I550" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J550" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K550" s="13" t="str">
         <f>IF(I550=J550,I550)</f>
-        <v>S</v>
-      </c>
+        <v>N</v>
+      </c>
+      <c r="L550" s="13"/>
       <c r="M550" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="551" spans="1:13" ht="87" x14ac:dyDescent="0.35">
-      <c r="A551" s="13">
-        <v>914</v>
-      </c>
-      <c r="B551" s="13" t="s">
-        <v>378</v>
-      </c>
-      <c r="C551" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D551" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E551" s="13">
-        <v>6</v>
-      </c>
-      <c r="F551" s="16" t="s">
-        <v>559</v>
-      </c>
-      <c r="G551" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="H551" s="16" t="s">
-        <v>560</v>
-      </c>
-      <c r="I551" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="J551" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="K551" s="4" t="str">
-        <f>IF(I551=J551,I551)</f>
-        <v>N</v>
-      </c>
-      <c r="M551" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="552" spans="1:13" ht="58" x14ac:dyDescent="0.35">
-      <c r="A552" s="13">
-        <v>931</v>
-      </c>
-      <c r="B552" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="C552" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D552" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E552" s="13">
-        <v>4</v>
-      </c>
-      <c r="F552" s="16" t="s">
-        <v>1281</v>
-      </c>
-      <c r="G552" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H552" s="16" t="s">
-        <v>1282</v>
-      </c>
-      <c r="I552" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J552" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K552" s="13" t="str">
-        <f>IF(I552=J552,I552)</f>
-        <v>L</v>
-      </c>
+        <f>IF(I550=J550,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="551" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A551" s="13"/>
+      <c r="B551" s="13"/>
+      <c r="C551" s="13"/>
+      <c r="D551" s="13"/>
+      <c r="E551" s="13"/>
+      <c r="F551" s="16"/>
+      <c r="G551" s="13"/>
+      <c r="H551" s="16"/>
+      <c r="I551" s="13"/>
+      <c r="J551" s="13"/>
+      <c r="K551" s="13"/>
+      <c r="L551" s="13"/>
+    </row>
+    <row r="552" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A552" s="13"/>
+      <c r="B552" s="13"/>
+      <c r="C552" s="13"/>
+      <c r="D552" s="13"/>
+      <c r="E552" s="13"/>
+      <c r="F552" s="16"/>
+      <c r="G552" s="13"/>
+      <c r="H552" s="16"/>
+      <c r="I552" s="13"/>
+      <c r="J552" s="13"/>
+      <c r="K552" s="13"/>
       <c r="L552" s="13"/>
-      <c r="M552" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="553" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A553" s="13">
-        <v>933</v>
-      </c>
-      <c r="B553" s="13" t="s">
-        <v>737</v>
-      </c>
-      <c r="C553" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D553" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E553" s="13">
-        <v>7</v>
-      </c>
-      <c r="F553" s="16" t="s">
-        <v>1283</v>
-      </c>
-      <c r="G553" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="H553" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="I553" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J553" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="K553" s="13" t="str">
-        <f>IF(I553=J553,I553)</f>
-        <v>N</v>
-      </c>
+    </row>
+    <row r="553" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A553" s="13"/>
+      <c r="B553" s="13"/>
+      <c r="C553" s="13"/>
+      <c r="D553" s="13"/>
+      <c r="E553" s="13"/>
+      <c r="F553" s="16"/>
+      <c r="G553" s="13"/>
+      <c r="H553" s="16"/>
+      <c r="I553" s="13"/>
+      <c r="J553" s="13"/>
+      <c r="K553" s="13"/>
       <c r="L553" s="13"/>
-      <c r="M553" s="11">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="554" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A554" s="13"/>
@@ -27244,53 +27203,11 @@
       <c r="K560" s="13"/>
       <c r="L560" s="13"/>
     </row>
-    <row r="561" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A561" s="13"/>
-      <c r="B561" s="13"/>
-      <c r="C561" s="13"/>
-      <c r="D561" s="13"/>
-      <c r="E561" s="13"/>
-      <c r="F561" s="16"/>
-      <c r="G561" s="13"/>
-      <c r="H561" s="16"/>
-      <c r="I561" s="13"/>
-      <c r="J561" s="13"/>
-      <c r="K561" s="13"/>
-      <c r="L561" s="13"/>
-    </row>
-    <row r="562" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A562" s="13"/>
-      <c r="B562" s="13"/>
-      <c r="C562" s="13"/>
-      <c r="D562" s="13"/>
-      <c r="E562" s="13"/>
-      <c r="F562" s="16"/>
-      <c r="G562" s="13"/>
-      <c r="H562" s="16"/>
-      <c r="I562" s="13"/>
-      <c r="J562" s="13"/>
-      <c r="K562" s="13"/>
-      <c r="L562" s="13"/>
-    </row>
-    <row r="563" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A563" s="13"/>
-      <c r="B563" s="13"/>
-      <c r="C563" s="13"/>
-      <c r="D563" s="13"/>
-      <c r="E563" s="13"/>
-      <c r="F563" s="16"/>
-      <c r="G563" s="13"/>
-      <c r="H563" s="16"/>
-      <c r="I563" s="13"/>
-      <c r="J563" s="13"/>
-      <c r="K563" s="13"/>
-      <c r="L563" s="13"/>
-    </row>
   </sheetData>
-  <sortState ref="A2:O549">
+  <sortState ref="A2:P563">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="K1 M1:M553">
+  <conditionalFormatting sqref="K1 M1:M550">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>